<commit_message>
2024.10.23 ruoqiang threshold update
</commit_message>
<xml_diff>
--- a/error_threshold/昆头岭金风故障阈值.xlsx
+++ b/error_threshold/昆头岭金风故障阈值.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView windowWidth="28800" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="故障阈值" sheetId="1" r:id="rId1"/>
@@ -1239,12 +1239,12 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.55752212389381" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.55833333333333" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17.8318584070796" customWidth="1"/>
+    <col min="1" max="1" width="17.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1269,11 +1269,9 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>70</v>
-      </c>
-      <c r="C2">
         <v>75</v>
       </c>
+      <c r="C2"/>
       <c r="D2">
         <v>80</v>
       </c>
@@ -1286,11 +1284,9 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>70</v>
-      </c>
-      <c r="C3">
         <v>75</v>
       </c>
+      <c r="C3"/>
       <c r="D3">
         <v>80</v>
       </c>

</xml_diff>